<commit_message>
Added average shap value plots to the train methods to see which features have the biggest impact
</commit_message>
<xml_diff>
--- a/Data/CorrelationMatrix.xlsx
+++ b/Data/CorrelationMatrix.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,11 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>RentalPriceAvg%Change</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>AnnualizedMoM-CPI-Inflation</t>
         </is>
       </c>
@@ -559,6 +564,9 @@
         <v>-0.04620955965928098</v>
       </c>
       <c r="P2" t="n">
+        <v>0.05889156954060009</v>
+      </c>
+      <c r="Q2" t="n">
         <v>0.2271087448552279</v>
       </c>
     </row>
@@ -611,6 +619,9 @@
         <v>-0.04524354284431157</v>
       </c>
       <c r="P3" t="n">
+        <v>-0.04067178712249819</v>
+      </c>
+      <c r="Q3" t="n">
         <v>0.104231386099139</v>
       </c>
     </row>
@@ -663,6 +674,9 @@
         <v>0.07592723447461534</v>
       </c>
       <c r="P4" t="n">
+        <v>-0.05064878077826373</v>
+      </c>
+      <c r="Q4" t="n">
         <v>0.1825749349860218</v>
       </c>
     </row>
@@ -715,6 +729,9 @@
         <v>0.09601369188684356</v>
       </c>
       <c r="P5" t="n">
+        <v>0.02935561778095505</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0.1122789910194018</v>
       </c>
     </row>
@@ -767,6 +784,9 @@
         <v>0.1384012863708351</v>
       </c>
       <c r="P6" t="n">
+        <v>0.1415789404803691</v>
+      </c>
+      <c r="Q6" t="n">
         <v>-0.02783271832262528</v>
       </c>
     </row>
@@ -819,6 +839,9 @@
         <v>0.07839265361012476</v>
       </c>
       <c r="P7" t="n">
+        <v>-0.02105499089153281</v>
+      </c>
+      <c r="Q7" t="n">
         <v>0.01738612832585752</v>
       </c>
     </row>
@@ -871,6 +894,9 @@
         <v>0.0608984187337203</v>
       </c>
       <c r="P8" t="n">
+        <v>0.1579867334488559</v>
+      </c>
+      <c r="Q8" t="n">
         <v>-0.06006850056062855</v>
       </c>
     </row>
@@ -923,6 +949,9 @@
         <v>0.186521088288075</v>
       </c>
       <c r="P9" t="n">
+        <v>-0.1071148522496317</v>
+      </c>
+      <c r="Q9" t="n">
         <v>0.2656560165021388</v>
       </c>
     </row>
@@ -975,6 +1004,9 @@
         <v>0.2017229594760396</v>
       </c>
       <c r="P10" t="n">
+        <v>-0.18170706190952</v>
+      </c>
+      <c r="Q10" t="n">
         <v>0.8814428604131235</v>
       </c>
     </row>
@@ -1027,6 +1059,9 @@
         <v>0.09948975402283593</v>
       </c>
       <c r="P11" t="n">
+        <v>-0.07659417116168638</v>
+      </c>
+      <c r="Q11" t="n">
         <v>0.02662536034064168</v>
       </c>
     </row>
@@ -1079,6 +1114,9 @@
         <v>0.1800627971240236</v>
       </c>
       <c r="P12" t="n">
+        <v>0.03118207290890015</v>
+      </c>
+      <c r="Q12" t="n">
         <v>0.05898536136485911</v>
       </c>
     </row>
@@ -1131,6 +1169,9 @@
         <v>-0.1090974766642365</v>
       </c>
       <c r="P13" t="n">
+        <v>-0.03672035828256448</v>
+      </c>
+      <c r="Q13" t="n">
         <v>-0.1628969161592023</v>
       </c>
     </row>
@@ -1183,6 +1224,9 @@
         <v>0.1824394418033169</v>
       </c>
       <c r="P14" t="n">
+        <v>0.04763660614841278</v>
+      </c>
+      <c r="Q14" t="n">
         <v>0.2196744218156774</v>
       </c>
     </row>
@@ -1235,58 +1279,119 @@
         <v>1</v>
       </c>
       <c r="P15" t="n">
+        <v>0.3399132241931659</v>
+      </c>
+      <c r="Q15" t="n">
         <v>0.3801215891929439</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
+          <t>RentalPriceAvg%Change</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.05889156954060009</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-0.04067178712249819</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.05064878077826373</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.02935561778095505</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.1415789404803691</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-0.02105499089153281</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.1579867334488559</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-0.1071148522496317</v>
+      </c>
+      <c r="J16" t="n">
+        <v>-0.18170706190952</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-0.07659417116168638</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.03118207290890015</v>
+      </c>
+      <c r="M16" t="n">
+        <v>-0.03672035828256448</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.04763660614841278</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.3399132241931659</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>-0.02500055734430478</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
           <t>AnnualizedMoM-CPI-Inflation</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="B17" t="n">
         <v>0.2271087448552279</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C17" t="n">
         <v>0.104231386099139</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D17" t="n">
         <v>0.1825749349860218</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E17" t="n">
         <v>0.1122789910194018</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F17" t="n">
         <v>-0.02783271832262528</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G17" t="n">
         <v>0.01738612832585752</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H17" t="n">
         <v>-0.06006850056062855</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I17" t="n">
         <v>0.2656560165021388</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J17" t="n">
         <v>0.8814428604131235</v>
       </c>
-      <c r="K16" t="n">
+      <c r="K17" t="n">
         <v>0.02662536034064168</v>
       </c>
-      <c r="L16" t="n">
+      <c r="L17" t="n">
         <v>0.05898536136485911</v>
       </c>
-      <c r="M16" t="n">
+      <c r="M17" t="n">
         <v>-0.1628969161592023</v>
       </c>
-      <c r="N16" t="n">
+      <c r="N17" t="n">
         <v>0.2196744218156774</v>
       </c>
-      <c r="O16" t="n">
+      <c r="O17" t="n">
         <v>0.3801215891929439</v>
       </c>
-      <c r="P16" t="n">
+      <c r="P17" t="n">
+        <v>-0.02500055734430478</v>
+      </c>
+      <c r="Q17" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reworked how the econ data is read and lagged in the code, created pre-2020 and 2020-beyond train/test/split
</commit_message>
<xml_diff>
--- a/Data/CorrelationMatrix.xlsx
+++ b/Data/CorrelationMatrix.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,11 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>2008-9RecessionDummyVar</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>AnnualizedMoM-CPI-Inflation</t>
         </is>
       </c>
@@ -567,6 +572,9 @@
         <v>0.05889156954060009</v>
       </c>
       <c r="Q2" t="n">
+        <v>-0.3040967956544474</v>
+      </c>
+      <c r="R2" t="n">
         <v>0.2271087448552279</v>
       </c>
     </row>
@@ -622,6 +630,9 @@
         <v>-0.04067178712249819</v>
       </c>
       <c r="Q3" t="n">
+        <v>-0.2014285535872592</v>
+      </c>
+      <c r="R3" t="n">
         <v>0.104231386099139</v>
       </c>
     </row>
@@ -677,6 +688,9 @@
         <v>-0.05064878077826373</v>
       </c>
       <c r="Q4" t="n">
+        <v>-0.2400181772862542</v>
+      </c>
+      <c r="R4" t="n">
         <v>0.1825749349860218</v>
       </c>
     </row>
@@ -732,6 +746,9 @@
         <v>0.02935561778095505</v>
       </c>
       <c r="Q5" t="n">
+        <v>-0.01743733957108285</v>
+      </c>
+      <c r="R5" t="n">
         <v>0.1122789910194018</v>
       </c>
     </row>
@@ -787,6 +804,9 @@
         <v>0.1415789404803691</v>
       </c>
       <c r="Q6" t="n">
+        <v>-0.01769392986876932</v>
+      </c>
+      <c r="R6" t="n">
         <v>-0.02783271832262528</v>
       </c>
     </row>
@@ -842,6 +862,9 @@
         <v>-0.02105499089153281</v>
       </c>
       <c r="Q7" t="n">
+        <v>0.04402117411545403</v>
+      </c>
+      <c r="R7" t="n">
         <v>0.01738612832585752</v>
       </c>
     </row>
@@ -897,6 +920,9 @@
         <v>0.1579867334488559</v>
       </c>
       <c r="Q8" t="n">
+        <v>-0.02468419043730151</v>
+      </c>
+      <c r="R8" t="n">
         <v>-0.06006850056062855</v>
       </c>
     </row>
@@ -952,6 +978,9 @@
         <v>-0.1071148522496317</v>
       </c>
       <c r="Q9" t="n">
+        <v>-0.03679216369613469</v>
+      </c>
+      <c r="R9" t="n">
         <v>0.2656560165021388</v>
       </c>
     </row>
@@ -1007,6 +1036,9 @@
         <v>-0.18170706190952</v>
       </c>
       <c r="Q10" t="n">
+        <v>-0.2677739025551792</v>
+      </c>
+      <c r="R10" t="n">
         <v>0.8814428604131235</v>
       </c>
     </row>
@@ -1062,6 +1094,9 @@
         <v>-0.07659417116168638</v>
       </c>
       <c r="Q11" t="n">
+        <v>0.03518189690949631</v>
+      </c>
+      <c r="R11" t="n">
         <v>0.02662536034064168</v>
       </c>
     </row>
@@ -1117,6 +1152,9 @@
         <v>0.03118207290890015</v>
       </c>
       <c r="Q12" t="n">
+        <v>-0.06424763057618306</v>
+      </c>
+      <c r="R12" t="n">
         <v>0.05898536136485911</v>
       </c>
     </row>
@@ -1172,6 +1210,9 @@
         <v>-0.03672035828256448</v>
       </c>
       <c r="Q13" t="n">
+        <v>0.04909288272459091</v>
+      </c>
+      <c r="R13" t="n">
         <v>-0.1628969161592023</v>
       </c>
     </row>
@@ -1227,6 +1268,9 @@
         <v>0.04763660614841278</v>
       </c>
       <c r="Q14" t="n">
+        <v>-0.1237936718063458</v>
+      </c>
+      <c r="R14" t="n">
         <v>0.2196744218156774</v>
       </c>
     </row>
@@ -1282,6 +1326,9 @@
         <v>0.3399132241931659</v>
       </c>
       <c r="Q15" t="n">
+        <v>0.1013215804987397</v>
+      </c>
+      <c r="R15" t="n">
         <v>0.3801215891929439</v>
       </c>
     </row>
@@ -1337,61 +1384,125 @@
         <v>1</v>
       </c>
       <c r="Q16" t="n">
+        <v>0.03525849430657787</v>
+      </c>
+      <c r="R16" t="n">
         <v>-0.02500055734430478</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
+          <t>2008-9RecessionDummyVar</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>-0.3040967956544474</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-0.2014285535872592</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.2400181772862542</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.01743733957108285</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-0.01769392986876932</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.04402117411545403</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-0.02468419043730151</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-0.03679216369613469</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-0.2677739025551792</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.03518189690949631</v>
+      </c>
+      <c r="L17" t="n">
+        <v>-0.06424763057618306</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.04909288272459091</v>
+      </c>
+      <c r="N17" t="n">
+        <v>-0.1237936718063458</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.1013215804987397</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.03525849430657787</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>1</v>
+      </c>
+      <c r="R17" t="n">
+        <v>-0.2932899553554737</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
           <t>AnnualizedMoM-CPI-Inflation</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="B18" t="n">
         <v>0.2271087448552279</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C18" t="n">
         <v>0.104231386099139</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D18" t="n">
         <v>0.1825749349860218</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E18" t="n">
         <v>0.1122789910194018</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F18" t="n">
         <v>-0.02783271832262528</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G18" t="n">
         <v>0.01738612832585752</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H18" t="n">
         <v>-0.06006850056062855</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I18" t="n">
         <v>0.2656560165021388</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J18" t="n">
         <v>0.8814428604131235</v>
       </c>
-      <c r="K17" t="n">
+      <c r="K18" t="n">
         <v>0.02662536034064168</v>
       </c>
-      <c r="L17" t="n">
+      <c r="L18" t="n">
         <v>0.05898536136485911</v>
       </c>
-      <c r="M17" t="n">
+      <c r="M18" t="n">
         <v>-0.1628969161592023</v>
       </c>
-      <c r="N17" t="n">
+      <c r="N18" t="n">
         <v>0.2196744218156774</v>
       </c>
-      <c r="O17" t="n">
+      <c r="O18" t="n">
         <v>0.3801215891929439</v>
       </c>
-      <c r="P17" t="n">
+      <c r="P18" t="n">
         <v>-0.02500055734430478</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="Q18" t="n">
+        <v>-0.2932899553554737</v>
+      </c>
+      <c r="R18" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>